<commit_message>
update hanya pake supremum
</commit_message>
<xml_diff>
--- a/rekomendasi.xlsx
+++ b/rekomendasi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,200 +434,29 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Method</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Nama Mobil</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Result</t>
-        </is>
+      <c r="A1" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Euclidean</t>
+          <t>Suzuki Ertiga</t>
         </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Daihatsu Xenia</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>4.321469612089302</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Euclidean</t>
+          <t>Xpander</t>
         </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Toyota Avanza</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.693822536363296</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Euclidean</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Toyota Agya</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>7.550337812777896</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Manhattan</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Daihatsu Xenia</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>7.580227743271221</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Manhattan</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Toyota Avanza</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>9.280538302277431</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Manhattan</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Toyota Agya</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>10.47308488612836</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Minkowski</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Daihatsu Xenia</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>137625.9367713193</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Minkowski</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Toyota Avanza</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>194955.0684261387</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Minkowski</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
           <t>Livina</t>
         </is>
-      </c>
-      <c r="C10" t="n">
-        <v>23472110.76440258</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Supremum</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Toyota Avanza</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>3.285714285714286</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Supremum</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Daihatsu Xenia</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>3.285714285714286</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Supremum</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Xpander</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>4.714285714285714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>